<commit_message>
Veritabanı kodları eklendi ve kodlar güncellendi
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Banka Kodu</t>
   </si>
@@ -35,13 +35,14 @@
     <t>00372</t>
   </si>
   <si>
-    <t>666009999</t>
+    <t xml:space="preserve">666009999       +</t>
   </si>
   <si>
     <t>255201,57</t>
   </si>
   <si>
-    <t>DBS Aktarım - DBS Aktarım</t>
+    <t>- DBS Aktar�m - DBS Aktar�m</t>
   </si>
 </sst>
 </file>
@@ -86,7 +87,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -126,23 +127,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>